<commit_message>
describe time left algorithm
</commit_message>
<xml_diff>
--- a/doc/TimeLeftAlgorithm.xlsx
+++ b/doc/TimeLeftAlgorithm.xlsx
@@ -372,7 +372,7 @@
   <dimension ref="H4:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,7 +382,7 @@
         <v>3</v>
       </c>
       <c r="R4">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="8:18" x14ac:dyDescent="0.25">
@@ -401,341 +401,281 @@
     </row>
     <row r="11" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H11">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="I11">
         <f>MOD(H11,$R$4)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="L11">
         <f>MOD(($R$4-I11+1),$R$4)</f>
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H12">
         <f>H11+1</f>
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I12">
         <f t="shared" ref="I12:I30" si="0">MOD(H12,$R$4)</f>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="L12">
         <f t="shared" ref="L12:L30" si="1">MOD(($R$4-I12+1),$R$4)</f>
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H13">
         <f t="shared" ref="H13:H30" si="2">H12+1</f>
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
         <v>2</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="N13">
-        <v>9</v>
       </c>
     </row>
     <row r="14" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="N14">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H15">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="N15">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H16">
         <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
         <v>5</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="N16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H17">
-        <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="N17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H18">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="N18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H19">
-        <f t="shared" si="2"/>
-        <v>38</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="N19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H20">
-        <f t="shared" si="2"/>
-        <v>39</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="N20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H21">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H22">
-        <f t="shared" si="2"/>
-        <v>41</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H23">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="N23">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H24">
-        <f t="shared" si="2"/>
-        <v>43</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="N24">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H25">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="N25">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H26">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="N26">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H27">
-        <f t="shared" si="2"/>
-        <v>46</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="N27">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H28">
-        <f t="shared" si="2"/>
-        <v>47</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="N28">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H29">
-        <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="N29">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H30">
-        <f t="shared" si="2"/>
-        <v>49</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="N30">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>